<commit_message>
fix extra time sum
</commit_message>
<xml_diff>
--- a/public/output/personel-29/پرسنل29_آبان_1400.xlsx
+++ b/public/output/personel-29/پرسنل29_آبان_1400.xlsx
@@ -269,7 +269,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -304,17 +304,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>